<commit_message>
Without Dead at 874
</commit_message>
<xml_diff>
--- a/ICP 1.0 JHall Mam Data.xlsx
+++ b/ICP 1.0 JHall Mam Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfh0044\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F26511-61C6-4B37-9ADA-C6F8272C143F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90021AC-9617-4DCC-982A-B9CD196C59C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{E37FFA8D-AE1C-4E0E-B1A8-E60F582325EA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{E37FFA8D-AE1C-4E0E-B1A8-E60F582325EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Actual Points Sampled" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5576" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5575" uniqueCount="444">
   <si>
     <t>WMA Name</t>
   </si>
@@ -15188,8 +15188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C628DB-8134-40E1-B822-69ADFB4657D1}">
   <dimension ref="A1:M957"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C862" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="M876" sqref="M876"/>
+    <sheetView tabSelected="1" topLeftCell="D862" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="L874" sqref="L874"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -47813,7 +47813,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="865" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="865" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A865" s="4" t="s">
         <v>90</v>
       </c>
@@ -47851,7 +47851,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="866" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="866" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A866" s="4" t="s">
         <v>90</v>
       </c>
@@ -47889,7 +47889,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="867" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="867" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A867" s="4" t="s">
         <v>90</v>
       </c>
@@ -47927,7 +47927,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="868" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="868" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A868" s="4" t="s">
         <v>300</v>
       </c>
@@ -47965,7 +47965,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="869" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="869" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A869" s="4" t="s">
         <v>300</v>
       </c>
@@ -48003,7 +48003,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="870" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="870" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A870" s="4" t="s">
         <v>300</v>
       </c>
@@ -48039,7 +48039,7 @@
       </c>
       <c r="L870" s="12"/>
     </row>
-    <row r="871" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="871" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A871" s="4" t="s">
         <v>300</v>
       </c>
@@ -48075,7 +48075,7 @@
       </c>
       <c r="L871" s="12"/>
     </row>
-    <row r="872" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="872" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A872" s="4" t="s">
         <v>300</v>
       </c>
@@ -48111,7 +48111,7 @@
       </c>
       <c r="L872" s="12"/>
     </row>
-    <row r="873" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="873" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A873" s="4" t="s">
         <v>300</v>
       </c>
@@ -48147,7 +48147,7 @@
       </c>
       <c r="L873" s="12"/>
     </row>
-    <row r="874" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="874" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A874" s="4" t="s">
         <v>302</v>
       </c>
@@ -48182,11 +48182,8 @@
         <v>56</v>
       </c>
       <c r="L874" s="12"/>
-      <c r="M874" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="875" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="875" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A875" s="4" t="s">
         <v>302</v>
       </c>
@@ -48222,7 +48219,7 @@
       </c>
       <c r="L875" s="12"/>
     </row>
-    <row r="876" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="876" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A876" s="4" t="s">
         <v>302</v>
       </c>
@@ -48258,7 +48255,7 @@
       </c>
       <c r="L876" s="12"/>
     </row>
-    <row r="877" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="877" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A877" s="4" t="s">
         <v>302</v>
       </c>
@@ -48294,7 +48291,7 @@
       </c>
       <c r="L877" s="12"/>
     </row>
-    <row r="878" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="878" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A878" s="4" t="s">
         <v>302</v>
       </c>
@@ -48330,7 +48327,7 @@
       </c>
       <c r="L878" s="12"/>
     </row>
-    <row r="879" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="879" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A879" s="4" t="s">
         <v>306</v>
       </c>
@@ -48366,7 +48363,7 @@
       </c>
       <c r="L879" s="12"/>
     </row>
-    <row r="880" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="880" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A880" s="4" t="s">
         <v>306</v>
       </c>
@@ -51279,14 +51276,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="168e4e8f-1310-4242-b1cf-13eb423cb96a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="32f715a4-5e4c-4cdc-a8e5-12fc608966dc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -51513,21 +51508,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="168e4e8f-1310-4242-b1cf-13eb423cb96a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="32f715a4-5e4c-4cdc-a8e5-12fc608966dc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F434993-5D14-4B46-AB23-E64DB1AB627C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{876B5226-4A2D-44A6-94B4-E351B4B193EB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="168e4e8f-1310-4242-b1cf-13eb423cb96a"/>
-    <ds:schemaRef ds:uri="32f715a4-5e4c-4cdc-a8e5-12fc608966dc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -51552,9 +51546,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{876B5226-4A2D-44A6-94B4-E351B4B193EB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F434993-5D14-4B46-AB23-E64DB1AB627C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="168e4e8f-1310-4242-b1cf-13eb423cb96a"/>
+    <ds:schemaRef ds:uri="32f715a4-5e4c-4cdc-a8e5-12fc608966dc"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>